<commit_message>
Updated the way to load pos and neg training images
</commit_message>
<xml_diff>
--- a/project/Calculations.xlsx
+++ b/project/Calculations.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UK\Documents\MATLAB\ML-Project\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UK\Documents\GitHub\Studium\ml-project\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>height</t>
   </si>
@@ -33,14 +34,107 @@
   </si>
   <si>
     <t>ratio</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>max_a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max_a=log_{q}(q+x) </t>
+  </si>
+  <si>
+    <t>(q+x)=q^max_a</t>
+  </si>
+  <si>
+    <t>x=q^max_a-q</t>
+  </si>
+  <si>
+    <t>rand</t>
+  </si>
+  <si>
+    <t>a=log_{q+y}(q+x)</t>
+  </si>
+  <si>
+    <t>a is max for y=0</t>
+  </si>
+  <si>
+    <t>hyper-parameter</t>
+  </si>
+  <si>
+    <t>random</t>
+  </si>
+  <si>
+    <t>a=log_{q+0,5*(q^max_a-q)}(q+q^max_a-q)</t>
+  </si>
+  <si>
+    <t>a=log_{0,5*(q^max_a+q)}(q^max_a)</t>
+  </si>
+  <si>
+    <t>a=ln(q^max_a)/ln(0,5*(q^max_a+q))</t>
+  </si>
+  <si>
+    <t>a=max_a*ln(q)/(ln(0,5)+ln(q^max_a+q))</t>
+  </si>
+  <si>
+    <t>TODO maybe construct a method that considers hyper-parameters of the scanning through the image when testing the model</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>q=1+b/(max_a-1)</t>
+  </si>
+  <si>
+    <t>y=(1-rand)*x</t>
+  </si>
+  <si>
+    <t>a_0,5</t>
+  </si>
+  <si>
+    <t>a -&gt; a': 1 -&gt; 1, max_a -&gt; max_a, a_0,5=(1+max_a)/2 should be reached by rand=0,5</t>
+  </si>
+  <si>
+    <t>Math.log(useLowerValues*prob + 1) / Math.log(useLowerValues*maxProb + 1))</t>
+  </si>
+  <si>
+    <t>useLowerValues = 100;</t>
+  </si>
+  <si>
+    <t>p</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -68,8 +162,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -352,7 +450,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="J5:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
@@ -472,4 +570,203 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C2:J30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>0.5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <f>1+D3/(D2-1)</f>
+        <v>1.5263157894736841</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <f>D6^D2-D6</f>
+        <v>4707.0318413746118</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <f>(1-D4)*D7</f>
+        <v>2353.5159206873059</v>
+      </c>
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="3">
+        <f>LOG(D6+D7,2)/LOG(D6+D8,2)</f>
+        <v>1.0892317184180225</v>
+      </c>
+      <c r="F10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="4">
+        <f>(1+D2)/2</f>
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J12" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C19" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29">
+        <f>LOG10(D27*D25+1)/LOG10(D27+1)</f>
+        <v>0.85194430316099234</v>
+      </c>
+    </row>
+    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30">
+        <f>1+(1-D29)*(D26-1)</f>
+        <v>2.3325012715510689</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>